<commit_message>
update practical distributions and sensitivity with 5 SD for LI
</commit_message>
<xml_diff>
--- a/data/data_out/v2023/macro_nutrients_concentrations.xlsx
+++ b/data/data_out/v2023/macro_nutrients_concentrations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="126" uniqueCount="3">
   <si>
     <t>Xch</t>
   </si>
@@ -79,9 +79,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="11.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -657,9 +657,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="11.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -740,9 +740,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="11.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -878,9 +878,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -939,9 +939,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1231,9 +1231,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1314,9 +1314,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="11.5546875" customWidth="true"/>
+    <col min="1" max="1" width="12.42578125" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>